<commit_message>
upload new versions of excel workbooks
</commit_message>
<xml_diff>
--- a/images/IntroExcel-Part2-SampleTestaMacroWorkbook.xlsx
+++ b/images/IntroExcel-Part2-SampleTestaMacroWorkbook.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t>Title</t>
-  </si>
-  <si>
-    <t>Title_Remark</t>
   </si>
   <si>
     <t>Author</t>
@@ -969,16 +966,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -997,408 +991,405 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="D2">
+        <v>2018</v>
       </c>
       <c r="E2">
+        <v>9781315298696</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>2017</v>
+      </c>
+      <c r="E3">
+        <v>9781137550743</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
         <v>2018</v>
       </c>
-      <c r="F2">
-        <v>9781315298696</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>2017</v>
-      </c>
-      <c r="F3">
-        <v>9781137550743</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E4">
+        <v>9783319766997</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
         <v>2018</v>
       </c>
-      <c r="F4">
-        <v>9783319766997</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E5">
+        <v>9783319764900</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
+      <c r="D6">
         <v>2018</v>
       </c>
-      <c r="F5">
-        <v>9783319764900</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E6">
+        <v>9783319774169</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6">
-        <v>2018</v>
-      </c>
-      <c r="F6">
-        <v>9783319774169</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7">
+        <v>2014</v>
+      </c>
+      <c r="E7">
+        <v>9783839426104</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="E7">
-        <v>2014</v>
-      </c>
-      <c r="F7">
-        <v>9783839426104</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8">
+        <v>2017</v>
+      </c>
+      <c r="E8">
+        <v>9780812293951</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="E8">
-        <v>2017</v>
-      </c>
-      <c r="F8">
-        <v>9780812293951</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9">
+        <v>2018</v>
+      </c>
+      <c r="E9">
+        <v>9780231545891</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="E9">
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
         <v>2018</v>
       </c>
-      <c r="F9">
-        <v>9780231545891</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E10">
+        <v>9781315439464</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10">
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
         <v>2018</v>
       </c>
-      <c r="F10">
-        <v>9781315439464</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E11">
+        <v>9783319899329</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11">
-        <v>2018</v>
-      </c>
-      <c r="F11">
-        <v>9783319899329</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12">
+        <v>2018</v>
+      </c>
+      <c r="E12">
+        <v>9781440852756</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="E12">
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
         <v>2018</v>
       </c>
-      <c r="F12">
-        <v>9781440852756</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E13">
+        <v>9783319760117</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13">
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>2016</v>
+      </c>
+      <c r="E14">
+        <v>9783839436165</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15">
+        <v>2016</v>
+      </c>
+      <c r="E15">
+        <v>9781447317388</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16">
+        <v>2015</v>
+      </c>
+      <c r="E16">
+        <v>9783839425169</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <v>2017</v>
+      </c>
+      <c r="E17">
+        <v>9780231544719</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18">
+        <v>2016</v>
+      </c>
+      <c r="E18">
+        <v>9780812292404</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19">
         <v>2018</v>
       </c>
-      <c r="F13">
-        <v>9783319760117</v>
-      </c>
-      <c r="G13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14">
+      <c r="E19">
+        <v>9781351254700</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20">
+        <v>2014</v>
+      </c>
+      <c r="E20">
+        <v>9783839420430</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21">
         <v>2016</v>
       </c>
-      <c r="F14">
-        <v>9783839436165</v>
-      </c>
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15">
-        <v>2016</v>
-      </c>
-      <c r="F15">
-        <v>9781447317388</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16">
-        <v>2015</v>
-      </c>
-      <c r="F16">
-        <v>9783839425169</v>
-      </c>
-      <c r="G16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17">
-        <v>2017</v>
-      </c>
-      <c r="F17">
-        <v>9780231544719</v>
-      </c>
-      <c r="G17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18">
-        <v>2016</v>
-      </c>
-      <c r="F18">
-        <v>9780812292404</v>
-      </c>
-      <c r="G18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19">
+      <c r="E21">
+        <v>9783839431115</v>
+      </c>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22">
         <v>2018</v>
       </c>
-      <c r="F19">
-        <v>9781351254700</v>
-      </c>
-      <c r="G19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20">
-        <v>2014</v>
-      </c>
-      <c r="F20">
-        <v>9783839420430</v>
-      </c>
-      <c r="G20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21">
-        <v>2016</v>
-      </c>
-      <c r="F21">
-        <v>9783839431115</v>
-      </c>
-      <c r="G21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22">
+        <v>9781108633208</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>43</v>
       </c>
-      <c r="E22">
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23">
         <v>2018</v>
       </c>
-      <c r="F22">
-        <v>9781108633208</v>
-      </c>
-      <c r="G22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23">
+        <v>9781439914731</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="E23">
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24">
         <v>2018</v>
       </c>
-      <c r="F23">
-        <v>9781439914731</v>
-      </c>
-      <c r="G23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" t="s">
-        <v>47</v>
-      </c>
       <c r="E24">
-        <v>2018</v>
-      </c>
-      <c r="F24">
         <v>9781785339073</v>
       </c>
-      <c r="G24" t="s">
-        <v>9</v>
+      <c r="F24" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upload updated excel files
</commit_message>
<xml_diff>
--- a/images/IntroExcel-Part2-SampleTestaMacroWorkbook.xlsx
+++ b/images/IntroExcel-Part2-SampleTestaMacroWorkbook.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
   <si>
     <t>Title</t>
   </si>
@@ -39,127 +39,247 @@
     <t>Binding</t>
   </si>
   <si>
-    <t>COLLECTIVE MEMORY WORK: A METHODOLOGY FOR LEARNING WITH AND FROM LIVED EXPERIENCE</t>
-  </si>
-  <si>
     <t>ROUTLEDGE</t>
   </si>
   <si>
-    <t>eBook</t>
-  </si>
-  <si>
-    <t>COMPASSIONATE MIGRATION AND REGIONAL POLICY IN THE AMERICAS</t>
-  </si>
-  <si>
-    <t>PALGRAVE MACMILLAN</t>
-  </si>
-  <si>
-    <t>GENDERING NATIONALISM: INTERSECTIONS OF NATION, GENDER AND SEXUALITY</t>
-  </si>
-  <si>
-    <t>GRIDDED WORLDS: AN URBAN ANTHOLOGY</t>
-  </si>
-  <si>
-    <t>SPRINGER</t>
-  </si>
-  <si>
-    <t>HANDBOOK OF COMMUNITY MOVEMENTS AND LOCAL ORGANIZATIONS IN THE 21ST CENTURY</t>
-  </si>
-  <si>
-    <t>IMAGE POLITICS OF CLIMATE CHANGE: VISUALIZATIONS, IMAGINATIONS, DOCUMENTATIONS</t>
-  </si>
-  <si>
-    <t>TRANSCRIPT</t>
-  </si>
-  <si>
-    <t>IMMIGRATION AND METROPOLITAN REVITALIZATION IN THE UNITED ST.</t>
-  </si>
-  <si>
-    <t>DOMENIC VITIELLO</t>
-  </si>
-  <si>
-    <t>UNIV PENN PRESS</t>
-  </si>
-  <si>
-    <t>IMMIGRATION POLICY IN THE AGE OF PUNISHMENT: DETENTION, DEPORTATION, AND BORDER CONTROL.</t>
-  </si>
-  <si>
-    <t>COLUMBIA UNIVERSITY PRESS</t>
-  </si>
-  <si>
-    <t>LAND RIGHTS, BIODIVERSITY CONSERVATION AND JUSTICE: RETHINKING PARKS AND PEOPLE</t>
-  </si>
-  <si>
-    <t>MACHINE LEARNING TECHNIQUES FOR ONLINE SOCIAL NETWORKS</t>
-  </si>
-  <si>
-    <t>MODERN AMERICAN EXTREMISM AND DOMESTIC TERRORISM: AN ENCYCLOPEDIA OF EXTREMISTS AND EXTREMIST GROUPS.</t>
-  </si>
-  <si>
-    <t>BALLECK, BARRY J.,</t>
-  </si>
-  <si>
-    <t>ABC-CLIO</t>
-  </si>
-  <si>
-    <t>ON REPLACEMENT: CULTURAL, SOCIAL AND PSYCHOLOGICAL REPRESENTATIONS</t>
-  </si>
-  <si>
-    <t>ORGANIZING NETWORKS: AN ACTOR-NETWORK THEORY OF ORGANIZATIONS.</t>
-  </si>
-  <si>
-    <t>BELLIGER, ANDREA</t>
-  </si>
-  <si>
-    <t>POLITICS, POWER AND COMMUNITY DEVELOPMENT</t>
-  </si>
-  <si>
-    <t>POLICY PRESS</t>
-  </si>
-  <si>
-    <t>REVEALING TACIT KNOWLEDGE: EMBODIMENT AND EXPLICATION</t>
-  </si>
-  <si>
-    <t>TRANSCRIPT VERLAG</t>
-  </si>
-  <si>
-    <t>RURAL POVERTY IN THE UNITED STATES</t>
-  </si>
-  <si>
-    <t>SHARED PROSPERITY IN AMERICA'S COMMUNITIES</t>
-  </si>
-  <si>
-    <t>UNIV OF PENNSYLVANIA PR</t>
-  </si>
-  <si>
-    <t>SOCIAL THEORIES OF URBAN VIOLENCE IN THE GLOBAL SOUTH: TOWARDS SAFE AND INCLUSIVE CITIES</t>
-  </si>
-  <si>
-    <t>THICK SPACE.</t>
-  </si>
-  <si>
-    <t>TRANSCRIPT-VERLAG</t>
-  </si>
-  <si>
-    <t>URBAN TRANSFORMATIONS IN THE U.S.A.: SPACES, COMMUNITIES, REPRESENTATIONS</t>
-  </si>
-  <si>
-    <t>WHAT IS A SLAVE SOCIETY?: THE PRACTICE OF SLAVERY IN GLOBAL PERSPECTIVE</t>
-  </si>
-  <si>
     <t>CAMBRIDGE UNIV PRESS</t>
   </si>
   <si>
-    <t>WILDLIFE CRIME: FROM THEORY TO PRACTICE</t>
-  </si>
-  <si>
-    <t>TEMPLE UNIVERSITY PRESS</t>
-  </si>
-  <si>
-    <t>WORLDWIDE MOBILIZATIONS: CLASS STRUGGLES AND URBAN COMMONING</t>
-  </si>
-  <si>
     <t>BERGHAHN BOOKS</t>
+  </si>
+  <si>
+    <t>3D RECORDING, DOCUMENTATION AND MANAGEMENT OF CULTURAL HERITAGE</t>
+  </si>
+  <si>
+    <t>WHITTLES PUBLISHING</t>
+  </si>
+  <si>
+    <t>Cloth</t>
+  </si>
+  <si>
+    <t>AMERICA'S DIGITAL ARMY: GAMES AT WORK AND WAR.</t>
+  </si>
+  <si>
+    <t>UNIV OF NEBRASKA PRESS</t>
+  </si>
+  <si>
+    <t>ARCHAEOLOGY OF AMERICAN CEMETERIES AND GRAVEMARKERS.</t>
+  </si>
+  <si>
+    <t>UNIV PR OF FLORIDA</t>
+  </si>
+  <si>
+    <t>ARCHAEOLOGY OF AMERICAN CHILDHOOD AND ADOLESCENCE.</t>
+  </si>
+  <si>
+    <t>ARCHAEOLOGY OF IDENTITY AND DISSONANCE: CONTEXTS FOR A BRAVE NEW WORLD</t>
+  </si>
+  <si>
+    <t>ARCHAEOLOGY OF STRUCTURAL VIOLENCE: LIFE IN A TWENTIETH-CENTURY COAL TOWN.</t>
+  </si>
+  <si>
+    <t>ARCHAEOLOGY OF THE COLD WAR.</t>
+  </si>
+  <si>
+    <t>ARCHAEOLOGY OF THE NORTH AMERICAN FUR TRADE.</t>
+  </si>
+  <si>
+    <t>BATTLES AND MASSACRES ON THE SOUTHWESTERN FRONTIER: HISTORICAL AND ARCHAEOLOGICAL PERSPECTIVES.</t>
+  </si>
+  <si>
+    <t>UNIV OF OKLAHOMA PRESS</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>COMING MAN FROM CANTON: CHINESE EXPERIENCE IN MONTANA, 1862-1943.</t>
+  </si>
+  <si>
+    <t>CREATIVE REPRESENTATIONS OF PLACE.</t>
+  </si>
+  <si>
+    <t>CULTURAL NEGOTIATIONS: THE ROLE OF WOMEN IN THE FOUNDING OF AMERICANIST ARCHAEOLOGY.</t>
+  </si>
+  <si>
+    <t>DIASPORA, DISASTERS, AND THE COSMOS: RITUALS AND IMAGES.</t>
+  </si>
+  <si>
+    <t>CAROLINA ACADEMIC</t>
+  </si>
+  <si>
+    <t>DISLOCATING LABOUR: ANTHROPOLOGICAL RECONFIGURATIONS</t>
+  </si>
+  <si>
+    <t>WILEY-BLACKWELL</t>
+  </si>
+  <si>
+    <t>ELDORADO!: THE ARCHAEOLOGY OF GOLD MINING IN THE FAR NORTH</t>
+  </si>
+  <si>
+    <t>ETHNOGRAPHIES OF U.S. EMPIRE</t>
+  </si>
+  <si>
+    <t>DUKE UNIVERSITY PRESS</t>
+  </si>
+  <si>
+    <t>FUTURE IN RUINS: UNESCO, WORLD HERITAGE, AND THE DREAM OF PEACE.</t>
+  </si>
+  <si>
+    <t>OXFORD UNIVERSITY PRESS</t>
+  </si>
+  <si>
+    <t>HANDBOOK ON THE GEOGRAPHIES OF POWER</t>
+  </si>
+  <si>
+    <t>EDWARD ELGAR</t>
+  </si>
+  <si>
+    <t>HISTORICAL ARCHAEOLOGY THROUGH A WESTERN LENS</t>
+  </si>
+  <si>
+    <t>HOLDING ON: AFRICAN AMERICAN WOMEN SURVIVING HIV/AIDS.</t>
+  </si>
+  <si>
+    <t>MEXICANS IN ALASKA: AN ETHNOGRAPHY OF MOBILITY, PLACE, AND TRANSNATIONAL LIFE.</t>
+  </si>
+  <si>
+    <t>MINING ARCHAEOLOGY IN THE AMERICAN WEST: A VIEW FROM THE SILVER STATE.</t>
+  </si>
+  <si>
+    <t>NEW GEOSPATIAL APPROACHES TO THE ANTHROPOLOGICAL SCIENCES</t>
+  </si>
+  <si>
+    <t>UNIV OF NEW MEXICO PRESS</t>
+  </si>
+  <si>
+    <t>ON THE EDGE OF PURGATORY: AN ARCHAEOLOGY OF PLACE IN HISPANIC COLORADO.</t>
+  </si>
+  <si>
+    <t>RAISING CHILDREN: SURPRISING INSIGHTS FROM OTHER CULTURES.</t>
+  </si>
+  <si>
+    <t>SENSE AND ESSENCE: HERITAGE AND THE CULTURAL PRODUCTION OF THE REAL</t>
+  </si>
+  <si>
+    <t>SETTING THE TABLE: CERAMICS, DINING, AND CULTURAL EXCHANGE IN ANDALUCIA AND LA FLORIDA.</t>
+  </si>
+  <si>
+    <t>SHELLFISH FOR THE CELESTIAL EMPIRE: THE RISE AND FALL OF COMMERCIAL ABALONE FISHING IN CALIFORNIA.</t>
+  </si>
+  <si>
+    <t>UNIV OF UTAH PRESS</t>
+  </si>
+  <si>
+    <t>SITUATIONAL IDENTITIES ALONG THE RAIDING FRONTIER OF COLONIAL NEW MEXICO.</t>
+  </si>
+  <si>
+    <t>SLAVE WHO WOULD BE KING: ORAL TRADITION AND ARCHAEOLOGY OF THE RECENT PAST IN THE UPPER SENEGAL RIVER BASIN.</t>
+  </si>
+  <si>
+    <t>ARCHAEOPRESS</t>
+  </si>
+  <si>
+    <t>VIRGINIA CITY: SECRETS OF A WESTERN PAST.</t>
+  </si>
+  <si>
+    <t>ZOOARCHAEOLOGY AND FIELD ECOLOGY: A PHOTOGRAPHIC ATLAS.</t>
+  </si>
+  <si>
+    <t>EFSTRATIOS STYLIANIDIS</t>
+  </si>
+  <si>
+    <t>ROBERTSON ALLEN</t>
+  </si>
+  <si>
+    <t>SHERENE BAUGHER</t>
+  </si>
+  <si>
+    <t>JANE EVA BAXTER</t>
+  </si>
+  <si>
+    <t>DIANE F. GEORGE</t>
+  </si>
+  <si>
+    <t>MICHAEL ROLLER</t>
+  </si>
+  <si>
+    <t>TODD A HANSON</t>
+  </si>
+  <si>
+    <t>MICHAEL S. NASSANEY</t>
+  </si>
+  <si>
+    <t>RONALD K. WETHERINGTON</t>
+  </si>
+  <si>
+    <t>CHRIS W. MERRITT</t>
+  </si>
+  <si>
+    <t>ALISON BARNES</t>
+  </si>
+  <si>
+    <t>DAVID L. BROWMAN</t>
+  </si>
+  <si>
+    <t>PAMELA J. STEWART</t>
+  </si>
+  <si>
+    <t>PENELOPE HARVEY</t>
+  </si>
+  <si>
+    <t>CATHERINE HOLDER SPUDE</t>
+  </si>
+  <si>
+    <t>CAROLE MCGRANAHAN</t>
+  </si>
+  <si>
+    <t>LYNN MESKELL</t>
+  </si>
+  <si>
+    <t>MAT COLEMAN</t>
+  </si>
+  <si>
+    <t>MARK WARNER</t>
+  </si>
+  <si>
+    <t>ALYSON O'DANIEL</t>
+  </si>
+  <si>
+    <t>SARA KOMARNISKY</t>
+  </si>
+  <si>
+    <t>DONALD L. HARDESTY</t>
+  </si>
+  <si>
+    <t>ROBERT L. ANEMONE</t>
+  </si>
+  <si>
+    <t>BONNIE J. CLARK</t>
+  </si>
+  <si>
+    <t>DAVID F. LANCY</t>
+  </si>
+  <si>
+    <t>BIRGIT MEYER</t>
+  </si>
+  <si>
+    <t>KATHRYN L. NESS</t>
+  </si>
+  <si>
+    <t>TODD J. BRAJE</t>
+  </si>
+  <si>
+    <t>JUN U. SUNSERI</t>
+  </si>
+  <si>
+    <t>JEFFREY H. ALTSCHUL</t>
+  </si>
+  <si>
+    <t>RONALD M. JAMES</t>
+  </si>
+  <si>
+    <t>JACK M. BROUGHT</t>
   </si>
 </sst>
 </file>
@@ -966,7 +1086,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -994,405 +1114,646 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="E2">
-        <v>9781315298696</v>
+        <v>9781498763035</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>2017</v>
       </c>
       <c r="E3">
-        <v>9781137550743</v>
+        <v>9780803285293</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="E4">
-        <v>9783319766997</v>
+        <v>9780813049717</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E5">
-        <v>9783319764900</v>
+        <v>9780813056098</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E6">
-        <v>9783319774169</v>
+        <v>9780813056197</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
       <c r="D7">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="E7">
-        <v>9783839426104</v>
+        <v>9780813056081</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D8">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E8">
-        <v>9780812293951</v>
+        <v>9780813062839</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D9">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="E9">
-        <v>9780231545891</v>
+        <v>9780813061573</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
       <c r="D10">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="E10">
-        <v>9781315439464</v>
+        <v>9780806144405</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E11">
-        <v>9783319899329</v>
+        <v>9780803299788</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D12">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E12">
-        <v>9781440852756</v>
+        <v>9781138061828</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D13">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="E13">
-        <v>9783319760117</v>
+        <v>9780803243811</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
       <c r="D14">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="E14">
-        <v>9783839436165</v>
+        <v>9781611633986</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
       <c r="D15">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="E15">
-        <v>9781447317388</v>
+        <v>9781119508380</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D16">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="E16">
-        <v>9783839425169</v>
+        <v>9780803210998</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D17">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="E17">
-        <v>9780231544719</v>
+        <v>9781478000099</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="C18" t="s">
-        <v>36</v>
-      </c>
       <c r="D18">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="E18">
-        <v>9780812292404</v>
+        <v>9780190648343</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
         <v>37</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
       </c>
       <c r="D19">
         <v>2018</v>
       </c>
       <c r="E19">
-        <v>9781351254700</v>
+        <v>9781785365638</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D20">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="E20">
-        <v>9783839420430</v>
+        <v>9780803277281</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D21">
         <v>2016</v>
       </c>
       <c r="E21">
-        <v>9783839431115</v>
+        <v>9780803269613</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D22">
         <v>2018</v>
       </c>
       <c r="E22">
-        <v>9781108633208</v>
+        <v>9781496203649</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="D23">
-        <v>2018</v>
+        <v>2010</v>
       </c>
       <c r="E23">
-        <v>9781439914731</v>
+        <v>9780803224407</v>
       </c>
       <c r="F23" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D24">
         <v>2018</v>
       </c>
       <c r="E24">
-        <v>9781785339073</v>
+        <v>9780826359674</v>
       </c>
       <c r="F24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>2011</v>
+      </c>
+      <c r="E25">
+        <v>9780803213722</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>2017</v>
+      </c>
+      <c r="E26">
+        <v>9781108415095</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
         <v>8</v>
+      </c>
+      <c r="D27">
+        <v>2018</v>
+      </c>
+      <c r="E27">
+        <v>9781785339394</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>2017</v>
+      </c>
+      <c r="E28">
+        <v>9781683400042</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29">
+        <v>2016</v>
+      </c>
+      <c r="E29">
+        <v>9781607814962</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>2017</v>
+      </c>
+      <c r="E30">
+        <v>9780803296398</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31">
+        <v>2016</v>
+      </c>
+      <c r="E31">
+        <v>9781784913519</v>
+      </c>
+      <c r="F31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>2012</v>
+      </c>
+      <c r="E32">
+        <v>9780803238480</v>
+      </c>
+      <c r="F32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33">
+        <v>2016</v>
+      </c>
+      <c r="E33">
+        <v>9781607814856</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>